<commit_message>
add feature to task
</commit_message>
<xml_diff>
--- a/patient_data.xlsx
+++ b/patient_data.xlsx
@@ -543,7 +543,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2378385</t>
+          <t>110508</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -593,7 +593,11 @@
         </is>
       </c>
       <c r="M2" t="inlineStr"/>
-      <c r="N2" t="inlineStr"/>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>01/04/2025</t>
+        </is>
+      </c>
       <c r="O2" t="inlineStr"/>
       <c r="P2" t="inlineStr">
         <is>
@@ -617,7 +621,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2380868</t>
+          <t>33997</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -663,7 +667,11 @@
         </is>
       </c>
       <c r="M3" t="inlineStr"/>
-      <c r="N3" t="inlineStr"/>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>02/04/2025</t>
+        </is>
+      </c>
       <c r="O3" t="inlineStr"/>
       <c r="P3" t="inlineStr">
         <is>
@@ -687,7 +695,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2376804</t>
+          <t>83868</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -737,7 +745,11 @@
         </is>
       </c>
       <c r="M4" t="inlineStr"/>
-      <c r="N4" t="inlineStr"/>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>01/04/2025</t>
+        </is>
+      </c>
       <c r="O4" t="inlineStr"/>
       <c r="P4" t="inlineStr">
         <is>
@@ -761,7 +773,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2309997</t>
+          <t>92999</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -811,7 +823,11 @@
         </is>
       </c>
       <c r="M5" t="inlineStr"/>
-      <c r="N5" t="inlineStr"/>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>31/03/2025</t>
+        </is>
+      </c>
       <c r="O5" t="inlineStr"/>
       <c r="P5" t="inlineStr">
         <is>
@@ -835,7 +851,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2381041</t>
+          <t>107585</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -881,7 +897,11 @@
         </is>
       </c>
       <c r="M6" t="inlineStr"/>
-      <c r="N6" t="inlineStr"/>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>01/04/2025</t>
+        </is>
+      </c>
       <c r="O6" t="inlineStr"/>
       <c r="P6" t="inlineStr">
         <is>
@@ -905,7 +925,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2378338</t>
+          <t>133674</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -955,7 +975,11 @@
         </is>
       </c>
       <c r="M7" t="inlineStr"/>
-      <c r="N7" t="inlineStr"/>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>01/04/2025</t>
+        </is>
+      </c>
       <c r="O7" t="inlineStr"/>
       <c r="P7" t="inlineStr">
         <is>
@@ -979,7 +1003,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2375071</t>
+          <t>52680</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -1029,7 +1053,11 @@
         </is>
       </c>
       <c r="M8" t="inlineStr"/>
-      <c r="N8" t="inlineStr"/>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>01/04/2025</t>
+        </is>
+      </c>
       <c r="O8" t="inlineStr"/>
       <c r="P8" t="inlineStr">
         <is>
@@ -1053,7 +1081,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>2375116</t>
+          <t>58017</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -1103,7 +1131,11 @@
         </is>
       </c>
       <c r="M9" t="inlineStr"/>
-      <c r="N9" t="inlineStr"/>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>01/04/2025</t>
+        </is>
+      </c>
       <c r="O9" t="inlineStr"/>
       <c r="P9" t="inlineStr">
         <is>
@@ -1127,7 +1159,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>2381164</t>
+          <t>132216</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -1173,7 +1205,11 @@
         </is>
       </c>
       <c r="M10" t="inlineStr"/>
-      <c r="N10" t="inlineStr"/>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>03/04/2025</t>
+        </is>
+      </c>
       <c r="O10" t="inlineStr"/>
       <c r="P10" t="inlineStr">
         <is>

</xml_diff>